<commit_message>
Added figures for ranking
</commit_message>
<xml_diff>
--- a/paper/resource/cross_validation_file_suppconf.xlsx
+++ b/paper/resource/cross_validation_file_suppconf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26518"/>
   <workbookPr date1904="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="2720" windowWidth="25360" windowHeight="15820" tabRatio="895" activeTab="6"/>
+    <workbookView xWindow="4100" yWindow="4980" windowWidth="25360" windowHeight="15820" tabRatio="895" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="minconf_table.csv" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>minconf</t>
   </si>
@@ -59,10 +59,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>recall</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>11items</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -79,10 +75,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>precision</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>recall</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -95,7 +87,23 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>MRR</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>Co-ref rules (confidence)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>recall</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>feedback</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>f-measure (recall)</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -103,7 +111,23 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>recall</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>f-measure (recall)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>Co-ref rules (support)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>feedback</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>f-measure (recall)</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -111,7 +135,23 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>recall</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>Co-ref rules (support*confidence)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>recall</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>feedback</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>f-measure (recall)</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -123,9 +163,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000%"/>
-    <numFmt numFmtId="177" formatCode="0.000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -187,7 +226,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="460">
+  <cellStyleXfs count="502">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -648,15 +687,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="437" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="437" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="437" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="460">
+  <cellStyles count="502">
     <cellStyle name="パーセント" xfId="437" builtinId="5"/>
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
@@ -887,6 +967,27 @@
     <cellStyle name="ハイパーリンク" xfId="454" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="456" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="476" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="498" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="500" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -1117,8 +1218,99 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="455" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="457" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="477" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="499" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="501" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1196,9 +1388,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.150100974639317"/>
-          <c:y val="0.0339561043241688"/>
+          <c:y val="0.369372703412073"/>
           <c:w val="0.787936205426551"/>
-          <c:h val="0.827245884037223"/>
+          <c:h val="0.491829232283464"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1871,11 +2063,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2131481704"/>
-        <c:axId val="-2131321160"/>
+        <c:axId val="-2055123224"/>
+        <c:axId val="-2064706664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2131481704"/>
+        <c:axId val="-2055123224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1943,7 +2135,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131321160"/>
+        <c:crossAx val="-2064706664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1951,7 +2143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131321160"/>
+        <c:axId val="-2064706664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +2191,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131481704"/>
+        <c:crossAx val="-2055123224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2013,6 +2205,37 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.183264844040418"/>
+          <c:y val="0.0166666666666667"/>
+          <c:w val="0.627032543678821"/>
+          <c:h val="0.321351541994751"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2419,11 +2642,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132751512"/>
-        <c:axId val="-2132745640"/>
+        <c:axId val="-2064699192"/>
+        <c:axId val="-2064847688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132751512"/>
+        <c:axId val="-2064699192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2472,7 +2695,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132745640"/>
+        <c:crossAx val="-2064847688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2480,7 +2703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132745640"/>
+        <c:axId val="-2064847688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2511,7 +2734,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132751512"/>
+        <c:crossAx val="-2064699192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -2927,11 +3150,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2134202344"/>
-        <c:axId val="-2145874568"/>
+        <c:axId val="-2068440936"/>
+        <c:axId val="-2013198200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2134202344"/>
+        <c:axId val="-2068440936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2980,7 +3203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145874568"/>
+        <c:crossAx val="-2013198200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2988,7 +3211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145874568"/>
+        <c:axId val="-2013198200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3019,7 +3242,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134202344"/>
+        <c:crossAx val="-2068440936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -4284,11 +4507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2128466952"/>
-        <c:axId val="-2128461480"/>
+        <c:axId val="-2064759624"/>
+        <c:axId val="-2054917000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2128466952"/>
+        <c:axId val="-2064759624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4336,13 +4559,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128461480"/>
+        <c:crossAx val="-2054917000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2128461480"/>
+        <c:axId val="-2054917000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -4361,13 +4584,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" altLang="ja-JP" sz="1800"/>
-                  <a:t>Precision</a:t>
+                  <a:t>MRR</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP" sz="1800" baseline="0"/>
-                  <a:t> (MRR)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1800"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4388,7 +4606,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128466952"/>
+        <c:crossAx val="-2064759624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -4400,10 +4618,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.186293276533338"/>
-          <c:y val="0.0746315137574095"/>
-          <c:w val="0.787885887878206"/>
-          <c:h val="0.283332035742723"/>
+          <c:x val="0.365894163451298"/>
+          <c:y val="0.0611483676899938"/>
+          <c:w val="0.599415821359359"/>
+          <c:h val="0.278837653720251"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4441,1015 +4659,6 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
-  <c:lang val="ja-JP"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.145800757721249"/>
-          <c:y val="0.0536924305452384"/>
-          <c:w val="0.814358293905058"/>
-          <c:h val="0.789907517456544"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Zimmermann graph (recall)'!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Co-ref rules (confidence)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="47625">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0443458980044346"/>
-                  <c:y val="0.0269662921348315"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.1</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0110866490912583"/>
-                  <c:y val="-0.00449438202247191"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.5</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0177385337919235"/>
-                  <c:y val="-0.0202247191011236"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.9</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Zimmermann graph (recall)'!$B$3:$J$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.331719038798804</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.283549637669567</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26288996153016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.229548793390029</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.200710241307971</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.169390803595883</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.117757660989947</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.108788258334117</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0997182424035591</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Zimmermann graph (recall)'!$B$2:$J$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.147491492237487</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.146237433616421</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.161057610652867</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.153019349545988</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.151054790008134</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.146011969699138</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.123263586143976</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.12182843762049</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.113698499697419</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Zimmermann graph (recall)'!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Co-ref rules (support)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="47625">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="star"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="47625" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0288248337028825"/>
-                  <c:y val="0.0134831460674157"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.1</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0332595980934756"/>
-                  <c:y val="0.0112359550561799"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.5</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0177383592017738"/>
-                  <c:y val="-0.00898894098911793"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.9</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Zimmermann graph (recall)'!$B$7:$J$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.331719038798804</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.283549637669567</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26288996153016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.229548793390029</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.200710241307971</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.169390803595883</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.117757660989947</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.108788258334117</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0997182424035591</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Zimmermann graph (recall)'!$B$6:$J$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.169750357244735</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.169542005721812</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.189651665827903</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.179515697511736</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.178928555108225</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.175738602729396</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.16294295839088</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.160904249064524</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.150991567925453</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Zimmermann graph (recall)'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Co-chg rules (confidence)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0443458980044346"/>
-                  <c:y val="0.0247191011235953"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.1</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0218525760776577"/>
-                  <c:y val="-0.0178699460320269"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.5</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0376940133037694"/>
-                  <c:y val="-0.0179775280898877"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.9</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Zimmermann graph (recall)'!$B$5:$J$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.223686243432691</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.186541009168176</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.145963421902291</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.11207207806792</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.083968060263149</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.063567346412174</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0424772113344513</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0332594874312331</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0224832215286103</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Zimmermann graph (recall)'!$B$4:$J$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.138881845000426</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.136796864944312</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15816813658845</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.148899002538551</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.153631641167084</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.157842386982864</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.159634594878945</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.164764144161363</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.219681128228736</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Zimmermann graph (recall)'!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Co-chg rules (support)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0266075388026607"/>
-                  <c:y val="0.0202247191011236"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.1</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0475635944620004"/>
-                  <c:y val="0.0192826683181455"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.5</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.0684719870104929"/>
-                  <c:y val="0.012796602671857"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US" altLang="ja-JP"/>
-                      <a:t>0.9</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Zimmermann graph (recall)'!$B$9:$J$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.223686243432691</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.186541009168176</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.145963421902291</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.11207207806792</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.083968060263149</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.063567346412174</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0424772113344513</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0332594874312331</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0224832215286103</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Zimmermann graph (recall)'!$B$8:$J$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.126822287327661</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.127309468312717</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.151889609838955</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.149096127870622</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.153709410061299</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.154258305500433</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.15452697979014</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.166141626264558</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.225516529362359</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2103200968"/>
-        <c:axId val="-2103248280"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="-2103200968"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0.0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1800"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP" sz="1800"/>
-                  <a:t>Recall</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.475032336644194"/>
-              <c:y val="0.915505617977528"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2103248280"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.1"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="-2103248280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="0.4"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1800"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP" sz="1800"/>
-                  <a:t>Precision</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP" sz="1800" baseline="0"/>
-                  <a:t> (MRR)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" altLang="ja-JP" sz="1800"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2103200968"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.1"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.186293276533338"/>
-          <c:y val="0.0746315137574095"/>
-          <c:w val="0.790103182778428"/>
-          <c:h val="0.211421923383173"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600"/>
-          </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="ja-JP"/>
@@ -6673,11 +5882,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127104280"/>
-        <c:axId val="-2127133000"/>
+        <c:axId val="-2064963672"/>
+        <c:axId val="-2064971320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127104280"/>
+        <c:axId val="-2064963672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -6725,13 +5934,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127133000"/>
+        <c:crossAx val="-2064971320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127133000"/>
+        <c:axId val="-2064971320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -6771,7 +5980,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127104280"/>
+        <c:crossAx val="-2064963672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -6823,7 +6032,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="ja-JP"/>
@@ -6845,9 +6054,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.173676931803016"/>
-          <c:y val="0.0615529063080598"/>
-          <c:w val="0.774099326037635"/>
-          <c:h val="0.80807860744935"/>
+          <c:y val="0.316963340647993"/>
+          <c:w val="0.778283365729911"/>
+          <c:h val="0.55266825868078"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -7524,11 +6733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2129656536"/>
-        <c:axId val="-2138775752"/>
+        <c:axId val="-2065021928"/>
+        <c:axId val="-2065024408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2129656536"/>
+        <c:axId val="-2065021928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7567,7 +6776,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138775752"/>
+        <c:crossAx val="-2065024408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7575,7 +6784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138775752"/>
+        <c:axId val="-2065024408"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -7621,7 +6830,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129656536"/>
+        <c:crossAx val="-2065021928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7635,6 +6844,41 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.253321716831325"/>
+          <c:y val="0.0245521304517786"/>
+          <c:w val="0.594569264647004"/>
+          <c:h val="0.264743068253909"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -7653,12 +6897,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:colOff>622300</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
@@ -7763,15 +7007,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>927100</xdr:colOff>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
+      <xdr:colOff>673100</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7787,38 +7031,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1651000</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7868,14 +7080,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>850900</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
@@ -8227,7 +7439,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J13"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -8266,7 +7478,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -8335,7 +7547,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0.33171903879880399</v>
@@ -8367,7 +7579,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>0.71655755067927096</v>
@@ -8399,7 +7611,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>0.204193075349237</v>
@@ -8431,7 +7643,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -8500,7 +7712,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>0.223686243432691</v>
@@ -8564,7 +7776,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>0.171366202267839</v>
@@ -8596,7 +7808,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -8665,7 +7877,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>0.33171903879880399</v>
@@ -8697,7 +7909,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>0.71655755067927096</v>
@@ -8729,7 +7941,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>0.224577714154617</v>
@@ -8761,7 +7973,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -8830,7 +8042,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>0.223686243432691</v>
@@ -8862,7 +8074,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>0.47654702571055302</v>
@@ -8926,7 +8138,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -8995,7 +8207,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>0.33171903879880399</v>
@@ -9027,7 +8239,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B30">
         <v>0.71655755067927096</v>
@@ -9059,7 +8271,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>0.23677876078410001</v>
@@ -9091,7 +8303,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -9160,7 +8372,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B35">
         <v>0.223686243432691</v>
@@ -9272,7 +8484,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9282,16 +8494,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -9299,13 +8511,13 @@
         <v>2E-3</v>
       </c>
       <c r="B2" s="3">
-        <v>0.5</v>
+        <v>1.222E-2</v>
       </c>
       <c r="C2" s="3">
+        <v>0.9748</v>
+      </c>
+      <c r="D2" s="3">
         <v>9.3790000000000002E-3</v>
-      </c>
-      <c r="D2" s="3">
-        <v>6.1700000000000004E-4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9313,13 +8525,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="B3" s="3">
-        <v>0.56830000000000003</v>
+        <v>6.1700000000000004E-4</v>
       </c>
       <c r="C3" s="3">
+        <v>0.129</v>
+      </c>
+      <c r="D3" s="3">
         <v>1.9949999999999998E-3</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2.0570000000000001E-5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -9327,18 +8539,18 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="B4" s="3">
-        <v>0.25919999999999999</v>
+        <v>9.4909999999999994E-3</v>
       </c>
       <c r="C4" s="3">
+        <v>2.997E-2</v>
+      </c>
+      <c r="D4" s="3">
         <v>1.4489999999999999E-2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3.4970000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -9346,6 +8558,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <conditionalFormatting sqref="B2:D4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.025</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -10343,17 +9560,17 @@
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -10373,8 +9590,8 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -10676,16 +9893,16 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="B2:J2">
-    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J3">
-    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:J4">
-    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:J5">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -10704,7 +9921,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -11005,6 +10222,24 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <conditionalFormatting sqref="B2:J2">
+    <cfRule type="top10" dxfId="6" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:J3">
+    <cfRule type="top10" dxfId="5" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:J4">
+    <cfRule type="top10" dxfId="4" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:J5">
+    <cfRule type="top10" dxfId="3" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:J6">
+    <cfRule type="top10" dxfId="2" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:J7">
+    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
@@ -11655,8 +10890,8 @@
   <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -12800,8 +12035,8 @@
   <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>